<commit_message>
deleted NoPlatform column in source and target file
</commit_message>
<xml_diff>
--- a/Source/06-01-2021 to 06-08-2021.xlsx
+++ b/Source/06-01-2021 to 06-08-2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangyulin/Bell program1/Source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangyulin/TVA_filter/Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A2E813-155F-0E46-8026-34C590E278E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117C3379-0730-9C41-8DF1-7E9DD9E00CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24680" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="60">
   <si>
     <t>TVA</t>
   </si>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t>8.9.0.36063-20201021</t>
-  </si>
-  <si>
-    <t>NoPlatform</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K160"/>
+  <dimension ref="A1:J160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1029,7 +1026,7 @@
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,11 +1057,8 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>8455700605838730</v>
       </c>
@@ -1095,11 +1089,8 @@
       <c r="J2">
         <v>16.48</v>
       </c>
-      <c r="K2">
-        <v>2893</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>5555555555555550</v>
       </c>
@@ -1130,11 +1121,8 @@
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>8455100605318120</v>
       </c>
@@ -1165,11 +1153,8 @@
       <c r="J4">
         <v>2.15</v>
       </c>
-      <c r="K4">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>8455800510469310</v>
       </c>
@@ -1200,11 +1185,8 @@
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>8455700624814480</v>
       </c>
@@ -1235,11 +1217,8 @@
       <c r="J6">
         <v>7.55</v>
       </c>
-      <c r="K6">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>8455800601627120</v>
       </c>
@@ -1270,11 +1249,8 @@
       <c r="J7">
         <v>1.39</v>
       </c>
-      <c r="K7">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>8455700606190690</v>
       </c>
@@ -1305,11 +1281,8 @@
       <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8455700604431630</v>
       </c>
@@ -1340,11 +1313,8 @@
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8455700500177650</v>
       </c>
@@ -1375,11 +1345,8 @@
       <c r="J10">
         <v>0.51</v>
       </c>
-      <c r="K10">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8445700510634760</v>
       </c>
@@ -1410,11 +1377,8 @@
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="K11">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -1445,11 +1409,8 @@
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>8455700604189270</v>
       </c>
@@ -1480,11 +1441,8 @@
       <c r="J13">
         <v>20.079999999999998</v>
       </c>
-      <c r="K13">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>8455700531554820</v>
       </c>
@@ -1515,11 +1473,8 @@
       <c r="J14">
         <v>0</v>
       </c>
-      <c r="K14">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>8455800510002050</v>
       </c>
@@ -1550,11 +1505,8 @@
       <c r="J15">
         <v>1.69</v>
       </c>
-      <c r="K15">
-        <v>12873</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1585,11 +1537,8 @@
       <c r="J16">
         <v>5.67</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>8455100633819600</v>
       </c>
@@ -1620,11 +1569,8 @@
       <c r="J17">
         <v>0</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>8455700511930240</v>
       </c>
@@ -1655,11 +1601,8 @@
       <c r="J18">
         <v>0.53</v>
       </c>
-      <c r="K18">
-        <v>332.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>8455800510126830</v>
       </c>
@@ -1690,11 +1633,8 @@
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>8455800601694460</v>
       </c>
@@ -1725,11 +1665,8 @@
       <c r="J20">
         <v>22.5</v>
       </c>
-      <c r="K20">
-        <v>32.799999999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>8455100665343950</v>
       </c>
@@ -1760,11 +1697,8 @@
       <c r="J21">
         <v>12.21</v>
       </c>
-      <c r="K21">
-        <v>32.799999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>8455800510429650</v>
       </c>
@@ -1795,11 +1729,8 @@
       <c r="J22">
         <v>27.79</v>
       </c>
-      <c r="K22">
-        <v>32.799999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1830,11 +1761,8 @@
       <c r="J23">
         <v>24.03</v>
       </c>
-      <c r="K23">
-        <v>32.799999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1865,11 +1793,8 @@
       <c r="J24">
         <v>0.25</v>
       </c>
-      <c r="K24">
-        <v>32.799999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>1.1111111111111101E+17</v>
       </c>
@@ -1900,11 +1825,8 @@
       <c r="J25">
         <v>0</v>
       </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>8455800510293910</v>
       </c>
@@ -1935,11 +1857,8 @@
       <c r="J26">
         <v>10.52</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>8455800510366410</v>
       </c>
@@ -1970,11 +1889,8 @@
       <c r="J27">
         <v>68.56</v>
       </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>8455700510533990</v>
       </c>
@@ -2005,11 +1921,8 @@
       <c r="J28">
         <v>6.81</v>
       </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>8455700607413190</v>
       </c>
@@ -2040,11 +1953,8 @@
       <c r="J29">
         <v>27.08</v>
       </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -2075,11 +1985,8 @@
       <c r="J30">
         <v>4.13</v>
       </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>8455700629360930</v>
       </c>
@@ -2110,11 +2017,8 @@
       <c r="J31">
         <v>0.84</v>
       </c>
-      <c r="K31">
-        <v>23.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>8455100501137450</v>
       </c>
@@ -2145,11 +2049,8 @@
       <c r="J32">
         <v>0.54</v>
       </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>8455800601362200</v>
       </c>
@@ -2180,11 +2081,8 @@
       <c r="J33">
         <v>14.63</v>
       </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>8455700605864500</v>
       </c>
@@ -2215,11 +2113,8 @@
       <c r="J34">
         <v>5.53</v>
       </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -2250,11 +2145,8 @@
       <c r="J35">
         <v>0.87</v>
       </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>8455700606106470</v>
       </c>
@@ -2285,11 +2177,8 @@
       <c r="J36">
         <v>18.350000000000001</v>
       </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>8455700510570030</v>
       </c>
@@ -2320,11 +2209,8 @@
       <c r="J37">
         <v>34.18</v>
       </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>8455700620975380</v>
       </c>
@@ -2355,11 +2241,8 @@
       <c r="J38">
         <v>53.92</v>
       </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>8455800510047700</v>
       </c>
@@ -2390,11 +2273,8 @@
       <c r="J39">
         <v>42.71</v>
       </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>8455800601570850</v>
       </c>
@@ -2425,11 +2305,8 @@
       <c r="J40">
         <v>25.71</v>
       </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>8455700625353750</v>
       </c>
@@ -2460,11 +2337,8 @@
       <c r="J41">
         <v>4.9400000000000004</v>
       </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>8455700600491820</v>
       </c>
@@ -2495,11 +2369,8 @@
       <c r="J42">
         <v>1.71</v>
       </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>8455100665672210</v>
       </c>
@@ -2530,11 +2401,8 @@
       <c r="J43">
         <v>32.9</v>
       </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>8455800603118630</v>
       </c>
@@ -2565,11 +2433,8 @@
       <c r="J44">
         <v>2.96</v>
       </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>8455700502285960</v>
       </c>
@@ -2600,11 +2465,8 @@
       <c r="J45">
         <v>3.32</v>
       </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>8455800500154570</v>
       </c>
@@ -2635,11 +2497,8 @@
       <c r="J46">
         <v>0</v>
       </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>8455700601001610</v>
       </c>
@@ -2670,11 +2529,8 @@
       <c r="J47">
         <v>0</v>
       </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2.22222222222222E+16</v>
       </c>
@@ -2705,11 +2561,8 @@
       <c r="J48">
         <v>0</v>
       </c>
-      <c r="K48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>8455700513241380</v>
       </c>
@@ -2740,11 +2593,8 @@
       <c r="J49">
         <v>0.49</v>
       </c>
-      <c r="K49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>8455700500176570</v>
       </c>
@@ -2775,11 +2625,8 @@
       <c r="J50">
         <v>3.55</v>
       </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>8455700601733240</v>
       </c>
@@ -2810,11 +2657,8 @@
       <c r="J51">
         <v>93.78</v>
       </c>
-      <c r="K51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>8455700510158740</v>
       </c>
@@ -2845,11 +2689,8 @@
       <c r="J52">
         <v>3.87</v>
       </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>8455700602268650</v>
       </c>
@@ -2880,11 +2721,8 @@
       <c r="J53">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>8455700515310610</v>
       </c>
@@ -2915,11 +2753,8 @@
       <c r="J54">
         <v>0</v>
       </c>
-      <c r="K54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>32</v>
       </c>
@@ -2950,11 +2785,8 @@
       <c r="J55">
         <v>0</v>
       </c>
-      <c r="K55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>8455800510454330</v>
       </c>
@@ -2985,11 +2817,8 @@
       <c r="J56">
         <v>14.45</v>
       </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>8455700628520600</v>
       </c>
@@ -3020,11 +2849,8 @@
       <c r="J57">
         <v>7.09</v>
       </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>8455700606476710</v>
       </c>
@@ -3055,11 +2881,8 @@
       <c r="J58">
         <v>34.03</v>
       </c>
-      <c r="K58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>8455800602429840</v>
       </c>
@@ -3090,11 +2913,8 @@
       <c r="J59">
         <v>9.5</v>
       </c>
-      <c r="K59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>8455700604973880</v>
       </c>
@@ -3125,11 +2945,8 @@
       <c r="J60">
         <v>5.87</v>
       </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>37</v>
       </c>
@@ -3160,11 +2977,8 @@
       <c r="J61">
         <v>82.28</v>
       </c>
-      <c r="K61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>3333333333</v>
       </c>
@@ -3195,11 +3009,8 @@
       <c r="J62">
         <v>0</v>
       </c>
-      <c r="K62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>8455800500141070</v>
       </c>
@@ -3230,11 +3041,8 @@
       <c r="J63">
         <v>0</v>
       </c>
-      <c r="K63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>8455800510154010</v>
       </c>
@@ -3265,11 +3073,8 @@
       <c r="J64">
         <v>27.34</v>
       </c>
-      <c r="K64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>8455800601938390</v>
       </c>
@@ -3300,11 +3105,8 @@
       <c r="J65">
         <v>8.93</v>
       </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>8455800510234840</v>
       </c>
@@ -3335,11 +3137,8 @@
       <c r="J66">
         <v>6.99</v>
       </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>8455700512475890</v>
       </c>
@@ -3370,11 +3169,8 @@
       <c r="J67">
         <v>2.63</v>
       </c>
-      <c r="K67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>8455800500119400</v>
       </c>
@@ -3405,11 +3201,8 @@
       <c r="J68">
         <v>0</v>
       </c>
-      <c r="K68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>8455700501356470</v>
       </c>
@@ -3440,11 +3233,8 @@
       <c r="J69">
         <v>0</v>
       </c>
-      <c r="K69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>8455700500354530</v>
       </c>
@@ -3475,11 +3265,8 @@
       <c r="J70">
         <v>0.84</v>
       </c>
-      <c r="K70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>8455700622984550</v>
       </c>
@@ -3510,11 +3297,8 @@
       <c r="J71">
         <v>0</v>
       </c>
-      <c r="K71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>39</v>
       </c>
@@ -3545,11 +3329,8 @@
       <c r="J72">
         <v>3.75</v>
       </c>
-      <c r="K72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>8455700605704580</v>
       </c>
@@ -3580,11 +3361,8 @@
       <c r="J73">
         <v>0.51</v>
       </c>
-      <c r="K73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>8455700607349140</v>
       </c>
@@ -3615,11 +3393,8 @@
       <c r="J74">
         <v>12.64</v>
       </c>
-      <c r="K74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>8455100602321820</v>
       </c>
@@ -3650,11 +3425,8 @@
       <c r="J75">
         <v>4.17</v>
       </c>
-      <c r="K75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>8455800601920500</v>
       </c>
@@ -3685,11 +3457,8 @@
       <c r="J76">
         <v>16.829999999999998</v>
       </c>
-      <c r="K76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>8455700510306170</v>
       </c>
@@ -3720,11 +3489,8 @@
       <c r="J77">
         <v>21.76</v>
       </c>
-      <c r="K77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>8455800601717560</v>
       </c>
@@ -3755,11 +3521,8 @@
       <c r="J78">
         <v>6.61</v>
       </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>8455800601094990</v>
       </c>
@@ -3790,11 +3553,8 @@
       <c r="J79">
         <v>112.54</v>
       </c>
-      <c r="K79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>8455700603176480</v>
       </c>
@@ -3825,11 +3585,8 @@
       <c r="J80">
         <v>0</v>
       </c>
-      <c r="K80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>8455800510000070</v>
       </c>
@@ -3860,11 +3617,8 @@
       <c r="J81">
         <v>90.77</v>
       </c>
-      <c r="K81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>8455800602429100</v>
       </c>
@@ -3895,11 +3649,8 @@
       <c r="J82">
         <v>0</v>
       </c>
-      <c r="K82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>41</v>
       </c>
@@ -3930,11 +3681,8 @@
       <c r="J83">
         <v>0</v>
       </c>
-      <c r="K83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>8455700606368940</v>
       </c>
@@ -3965,11 +3713,8 @@
       <c r="J84">
         <v>2.39</v>
       </c>
-      <c r="K84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>8455700625682600</v>
       </c>
@@ -4000,11 +3745,8 @@
       <c r="J85">
         <v>77.87</v>
       </c>
-      <c r="K85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>845570060103878</v>
       </c>
@@ -4035,11 +3777,8 @@
       <c r="J86">
         <v>0</v>
       </c>
-      <c r="K86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>8455800600993360</v>
       </c>
@@ -4070,11 +3809,8 @@
       <c r="J87">
         <v>0</v>
       </c>
-      <c r="K87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>8455700600057680</v>
       </c>
@@ -4105,11 +3841,8 @@
       <c r="J88">
         <v>0</v>
       </c>
-      <c r="K88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>8455700602314030</v>
       </c>
@@ -4140,11 +3873,8 @@
       <c r="J89">
         <v>1.78</v>
       </c>
-      <c r="K89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>8455700510543780</v>
       </c>
@@ -4175,11 +3905,8 @@
       <c r="J90">
         <v>47.29</v>
       </c>
-      <c r="K90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>42</v>
       </c>
@@ -4210,11 +3937,8 @@
       <c r="J91">
         <v>17.84</v>
       </c>
-      <c r="K91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>8455800500048940</v>
       </c>
@@ -4245,11 +3969,8 @@
       <c r="J92">
         <v>11.15</v>
       </c>
-      <c r="K92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>8455700606512770</v>
       </c>
@@ -4280,11 +4001,8 @@
       <c r="J93">
         <v>13.51</v>
       </c>
-      <c r="K93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>8455700600129120</v>
       </c>
@@ -4315,11 +4033,8 @@
       <c r="J94">
         <v>0</v>
       </c>
-      <c r="K94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>43</v>
       </c>
@@ -4350,11 +4065,8 @@
       <c r="J95">
         <v>0</v>
       </c>
-      <c r="K95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>8455800601459360</v>
       </c>
@@ -4385,11 +4097,8 @@
       <c r="J96">
         <v>14.55</v>
       </c>
-      <c r="K96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>8455100645767450</v>
       </c>
@@ -4420,11 +4129,8 @@
       <c r="J97">
         <v>21.66</v>
       </c>
-      <c r="K97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>8455700502592080</v>
       </c>
@@ -4455,11 +4161,8 @@
       <c r="J98">
         <v>49.32</v>
       </c>
-      <c r="K98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>8455700512154400</v>
       </c>
@@ -4490,11 +4193,8 @@
       <c r="J99">
         <v>0.61</v>
       </c>
-      <c r="K99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>8455800600440830</v>
       </c>
@@ -4525,11 +4225,8 @@
       <c r="J100">
         <v>21.45</v>
       </c>
-      <c r="K100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>8455800510239300</v>
       </c>
@@ -4560,11 +4257,8 @@
       <c r="J101">
         <v>40.11</v>
       </c>
-      <c r="K101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>8455800510441430</v>
       </c>
@@ -4595,11 +4289,8 @@
       <c r="J102">
         <v>0</v>
       </c>
-      <c r="K102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>8455100606126890</v>
       </c>
@@ -4630,11 +4321,8 @@
       <c r="J103">
         <v>0</v>
       </c>
-      <c r="K103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>8455800510049010</v>
       </c>
@@ -4665,11 +4353,8 @@
       <c r="J104">
         <v>13.16</v>
       </c>
-      <c r="K104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>8455800510243930</v>
       </c>
@@ -4700,11 +4385,8 @@
       <c r="J105">
         <v>41.92</v>
       </c>
-      <c r="K105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>8455800510349380</v>
       </c>
@@ -4735,11 +4417,8 @@
       <c r="J106">
         <v>2.57</v>
       </c>
-      <c r="K106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>8455700607496770</v>
       </c>
@@ -4770,11 +4449,8 @@
       <c r="J107">
         <v>12.2</v>
       </c>
-      <c r="K107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>8455700516136320</v>
       </c>
@@ -4805,11 +4481,8 @@
       <c r="J108">
         <v>0.78</v>
       </c>
-      <c r="K108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>8455700608313270</v>
       </c>
@@ -4840,11 +4513,8 @@
       <c r="J109">
         <v>24.9</v>
       </c>
-      <c r="K109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>8455800603168900</v>
       </c>
@@ -4875,11 +4545,8 @@
       <c r="J110">
         <v>4.08</v>
       </c>
-      <c r="K110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>8455700500043510</v>
       </c>
@@ -4910,11 +4577,8 @@
       <c r="J111">
         <v>0</v>
       </c>
-      <c r="K111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>8455100501501890</v>
       </c>
@@ -4945,11 +4609,8 @@
       <c r="J112">
         <v>0</v>
       </c>
-      <c r="K112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>8455800603443420</v>
       </c>
@@ -4980,11 +4641,8 @@
       <c r="J113">
         <v>3.46</v>
       </c>
-      <c r="K113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>8455100643437680</v>
       </c>
@@ -5015,11 +4673,8 @@
       <c r="J114">
         <v>27.85</v>
       </c>
-      <c r="K114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>8455800500281250</v>
       </c>
@@ -5050,11 +4705,8 @@
       <c r="J115">
         <v>0</v>
       </c>
-      <c r="K115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>8455700603000260</v>
       </c>
@@ -5085,11 +4737,8 @@
       <c r="J116">
         <v>13.73</v>
       </c>
-      <c r="K116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>48</v>
       </c>
@@ -5120,11 +4769,8 @@
       <c r="J117">
         <v>0.11</v>
       </c>
-      <c r="K117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>8455800601968570</v>
       </c>
@@ -5155,11 +4801,8 @@
       <c r="J118">
         <v>3.06</v>
       </c>
-      <c r="K118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>8455700600011920</v>
       </c>
@@ -5190,11 +4833,8 @@
       <c r="J119">
         <v>13.19</v>
       </c>
-      <c r="K119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>49</v>
       </c>
@@ -5225,11 +4865,8 @@
       <c r="J120">
         <v>0</v>
       </c>
-      <c r="K120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>8455800510334480</v>
       </c>
@@ -5260,11 +4897,8 @@
       <c r="J121">
         <v>17.13</v>
       </c>
-      <c r="K121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>8455700534724010</v>
       </c>
@@ -5295,11 +4929,8 @@
       <c r="J122">
         <v>0</v>
       </c>
-      <c r="K122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>8455700602256140</v>
       </c>
@@ -5330,11 +4961,8 @@
       <c r="J123">
         <v>0</v>
       </c>
-      <c r="K123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>8455700621419650</v>
       </c>
@@ -5365,11 +4993,8 @@
       <c r="J124">
         <v>5.17</v>
       </c>
-      <c r="K124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>8455800603051700</v>
       </c>
@@ -5400,11 +5025,8 @@
       <c r="J125">
         <v>2.67</v>
       </c>
-      <c r="K125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>8455700601403260</v>
       </c>
@@ -5435,11 +5057,8 @@
       <c r="J126">
         <v>0</v>
       </c>
-      <c r="K126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>8455800500000640</v>
       </c>
@@ -5470,11 +5089,8 @@
       <c r="J127">
         <v>75.05</v>
       </c>
-      <c r="K127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>51</v>
       </c>
@@ -5505,11 +5121,8 @@
       <c r="J128">
         <v>4.66</v>
       </c>
-      <c r="K128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>8455800600750510</v>
       </c>
@@ -5540,11 +5153,8 @@
       <c r="J129">
         <v>19.91</v>
       </c>
-      <c r="K129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>8455800601413790</v>
       </c>
@@ -5575,11 +5185,8 @@
       <c r="J130">
         <v>24.72</v>
       </c>
-      <c r="K130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>8455800510525490</v>
       </c>
@@ -5610,11 +5217,8 @@
       <c r="J131">
         <v>5.66</v>
       </c>
-      <c r="K131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>8455700510480510</v>
       </c>
@@ -5645,11 +5249,8 @@
       <c r="J132">
         <v>8.5399999999999991</v>
       </c>
-      <c r="K132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>8455800510546040</v>
       </c>
@@ -5680,11 +5281,8 @@
       <c r="J133">
         <v>0</v>
       </c>
-      <c r="K133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>8455700606852160</v>
       </c>
@@ -5715,11 +5313,8 @@
       <c r="J134">
         <v>9.6</v>
       </c>
-      <c r="K134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>8455700501356480</v>
       </c>
@@ -5750,11 +5345,8 @@
       <c r="J135">
         <v>198.79</v>
       </c>
-      <c r="K135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>8455800500216330</v>
       </c>
@@ -5785,11 +5377,8 @@
       <c r="J136">
         <v>23.48</v>
       </c>
-      <c r="K136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>8455800602055190</v>
       </c>
@@ -5820,11 +5409,8 @@
       <c r="J137">
         <v>13.04</v>
       </c>
-      <c r="K137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>8455700603581500</v>
       </c>
@@ -5855,11 +5441,8 @@
       <c r="J138">
         <v>8.6999999999999993</v>
       </c>
-      <c r="K138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>8455100648881260</v>
       </c>
@@ -5890,11 +5473,8 @@
       <c r="J139">
         <v>0</v>
       </c>
-      <c r="K139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>8455100620810060</v>
       </c>
@@ -5925,11 +5505,8 @@
       <c r="J140">
         <v>1.04</v>
       </c>
-      <c r="K140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>4444444444444</v>
       </c>
@@ -5960,11 +5537,8 @@
       <c r="J141">
         <v>0</v>
       </c>
-      <c r="K141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>8455700603348230</v>
       </c>
@@ -5995,11 +5569,8 @@
       <c r="J142">
         <v>81.58</v>
       </c>
-      <c r="K142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>8455100624299570</v>
       </c>
@@ -6030,11 +5601,8 @@
       <c r="J143">
         <v>0</v>
       </c>
-      <c r="K143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>8455700626290360</v>
       </c>
@@ -6065,11 +5633,8 @@
       <c r="J144">
         <v>2.0099999999999998</v>
       </c>
-      <c r="K144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>52</v>
       </c>
@@ -6100,11 +5665,8 @@
       <c r="J145">
         <v>0.1</v>
       </c>
-      <c r="K145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>8455700600099290</v>
       </c>
@@ -6135,11 +5697,8 @@
       <c r="J146">
         <v>1.81</v>
       </c>
-      <c r="K146">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>8455800602169970</v>
       </c>
@@ -6170,11 +5729,8 @@
       <c r="J147">
         <v>0</v>
       </c>
-      <c r="K147">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>8455700602318710</v>
       </c>
@@ -6205,11 +5761,8 @@
       <c r="J148">
         <v>12.49</v>
       </c>
-      <c r="K148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>8455700623067570</v>
       </c>
@@ -6240,11 +5793,8 @@
       <c r="J149">
         <v>72.06</v>
       </c>
-      <c r="K149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>8455800500262700</v>
       </c>
@@ -6275,11 +5825,8 @@
       <c r="J150">
         <v>0.02</v>
       </c>
-      <c r="K150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>56</v>
       </c>
@@ -6310,11 +5857,8 @@
       <c r="J151">
         <v>6.45</v>
       </c>
-      <c r="K151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>8455800600363730</v>
       </c>
@@ -6345,11 +5889,8 @@
       <c r="J152">
         <v>39.119999999999997</v>
       </c>
-      <c r="K152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>8455700600089300</v>
       </c>
@@ -6380,11 +5921,8 @@
       <c r="J153">
         <v>0</v>
       </c>
-      <c r="K153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>8455800600000130</v>
       </c>
@@ -6415,11 +5953,8 @@
       <c r="J154">
         <v>0</v>
       </c>
-      <c r="K154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>8455800603178000</v>
       </c>
@@ -6450,11 +5985,8 @@
       <c r="J155">
         <v>3.02</v>
       </c>
-      <c r="K155">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>8455800600000870</v>
       </c>
@@ -6485,11 +6017,8 @@
       <c r="J156">
         <v>62.88</v>
       </c>
-      <c r="K156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>8455800510307880</v>
       </c>
@@ -6520,11 +6049,8 @@
       <c r="J157">
         <v>4.07</v>
       </c>
-      <c r="K157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>8455800600046790</v>
       </c>
@@ -6555,11 +6081,8 @@
       <c r="J158">
         <v>4.57</v>
       </c>
-      <c r="K158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>58</v>
       </c>
@@ -6590,11 +6113,8 @@
       <c r="J159">
         <v>0.41</v>
       </c>
-      <c r="K159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B160">
         <v>0</v>
       </c>
@@ -6620,9 +6140,6 @@
         <v>0</v>
       </c>
       <c r="J160">
-        <v>0</v>
-      </c>
-      <c r="K160">
         <v>0</v>
       </c>
     </row>
@@ -6632,6 +6149,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -6681,28 +6207,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e6c45ce4-62b7-4548-be34-73524a8672bb">eSpW84482300-452014548-254</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e6c45ce4-62b7-4548-be34-73524a8672bb">
-      <Url>https://espace.int.bell.ca/workspaces/FONSE_Trial/_layouts/15/DocIdRedir.aspx?ID=eSpW84482300-452014548-254</Url>
-      <Description>eSpW84482300-452014548-254</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA4861948BA69B47BC3583A2272821AC" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b319bdd83d464ae759197631b79c89b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e6c45ce4-62b7-4548-be34-73524a8672bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d708c2205d10cac6721eaf5adcac72a7" ns2:_="">
     <xsd:import namespace="e6c45ce4-62b7-4548-be34-73524a8672bb"/>
@@ -6847,7 +6352,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e6c45ce4-62b7-4548-be34-73524a8672bb">eSpW84482300-452014548-254</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e6c45ce4-62b7-4548-be34-73524a8672bb">
+      <Url>https://espace.int.bell.ca/workspaces/FONSE_Trial/_layouts/15/DocIdRedir.aspx?ID=eSpW84482300-452014548-254</Url>
+      <Description>eSpW84482300-452014548-254</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA52D046-D993-4047-9126-66A86E3EED5C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{464E34F8-8CC0-4409-A823-560A79982274}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -6855,25 +6380,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA52D046-D993-4047-9126-66A86E3EED5C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F8E002-21DC-4FB3-B8B9-3070D3FF6F82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e6c45ce4-62b7-4548-be34-73524a8672bb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFE97B45-7A08-4455-B486-8F70F6B0BE86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6889,4 +6396,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F8E002-21DC-4FB3-B8B9-3070D3FF6F82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e6c45ce4-62b7-4548-be34-73524a8672bb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>